<commit_message>
Updated gantt file with progress and new requirement
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhagyeshrathi/Desktop/131_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marketplace_Project\Marketplace_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED84B044-C34A-CD4A-9B84-B5CE6D31235E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2EAD54-DA77-497B-A965-F54D83AA52F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="880" windowWidth="30420" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Feature 13</t>
-  </si>
-  <si>
     <t>Feature 14</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Buy Item-Bhagyesh/winson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget System </t>
   </si>
 </sst>
 </file>
@@ -274,17 +274,20 @@
       <sz val="13"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="7"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1067,18 +1070,18 @@
   <dimension ref="B1:BO30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="16" width="2.6640625" style="1"/>
-    <col min="17" max="17" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="27" width="2.6640625" style="1"/>
+    <col min="3" max="6" width="11.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" style="4" customWidth="1"/>
+    <col min="8" max="16" width="2.625" style="1"/>
+    <col min="17" max="17" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="27" width="2.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
@@ -1091,7 +1094,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
@@ -1149,7 +1152,7 @@
       <c r="AO2" s="24"/>
       <c r="AP2" s="24"/>
     </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="26" t="s">
         <v>14</v>
       </c>
@@ -1191,7 +1194,7 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27"/>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -1379,9 +1382,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
@@ -1399,9 +1402,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
@@ -1419,9 +1422,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
@@ -1439,9 +1442,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
@@ -1459,9 +1462,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
@@ -1479,9 +1482,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
@@ -1499,9 +1502,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="7">
         <v>2</v>
@@ -1519,9 +1522,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7">
         <v>3</v>
@@ -1539,9 +1542,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7">
         <v>5</v>
@@ -1559,9 +1562,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
         <v>3</v>
@@ -1579,9 +1582,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9">
         <v>3</v>
@@ -1599,9 +1602,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7">
         <v>6</v>
@@ -1619,29 +1622,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>15</v>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="C17" s="7">
         <v>9</v>
       </c>
       <c r="D17" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E17" s="7">
         <v>9</v>
       </c>
       <c r="F17" s="7">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G17" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="7">
         <v>9</v>
@@ -1659,9 +1662,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="7">
         <v>9</v>
@@ -1679,9 +1682,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -1699,9 +1702,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="7">
         <v>11</v>
@@ -1719,9 +1722,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="7">
         <v>12</v>
@@ -1739,9 +1742,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="7">
         <v>12</v>
@@ -1759,9 +1762,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="7">
         <v>14</v>
@@ -1779,9 +1782,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="7">
         <v>14</v>
@@ -1799,9 +1802,9 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="7">
         <v>14</v>
@@ -1819,9 +1822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="7">
         <v>15</v>
@@ -1839,9 +1842,9 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="7">
         <v>15</v>
@@ -1859,9 +1862,9 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="7">
         <v>15</v>
@@ -1879,9 +1882,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="7">
         <v>16</v>

</xml_diff>